<commit_message>
added PI and const U MPs
</commit_message>
<xml_diff>
--- a/Tables for paper/Table 2v2.xlsx
+++ b/Tables for paper/Table 2v2.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tcarruth\Documents\GitHub\AI-MP-EGB\Tables for paper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\AI-MP-EGB\Tables for paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB0FEB6-6551-4BA2-9970-0F616C9F50AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13123" windowHeight="6103" activeTab="1"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
     <sheet name="Formatted" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -186,7 +195,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -261,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -290,13 +299,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,21 +584,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="11.05078125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="6.07421875" customWidth="1"/>
-    <col min="3" max="3" width="7.15234375" customWidth="1"/>
+    <col min="2" max="2" width="6.05078125" customWidth="1"/>
+    <col min="3" max="3" width="7.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -616,7 +624,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -642,7 +650,7 @@
         <v>0.96334564180236104</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -668,7 +676,7 @@
         <v>0.97449145022429995</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -694,7 +702,7 @@
         <v>0.967328027030809</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -720,7 +728,7 @@
         <v>0.97009473637974497</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -746,7 +754,7 @@
         <v>0.97349800588123403</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -772,7 +780,7 @@
         <v>0.95788902945036902</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -798,7 +806,7 @@
         <v>0.96108029067035805</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -824,7 +832,7 @@
         <v>0.97189789350716604</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -850,7 +858,7 @@
         <v>0.97272178501889905</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -876,7 +884,7 @@
         <v>0.97182195896632495</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -902,7 +910,7 @@
         <v>0.96513272317718501</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -928,7 +936,7 @@
         <v>0.97694752227495796</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -954,7 +962,7 @@
         <v>0.96524418659858802</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -980,7 +988,7 @@
         <v>0.95918670197864697</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1006,7 +1014,7 @@
         <v>0.97181401875989903</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -1032,7 +1040,7 @@
         <v>0.97553076110830195</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1058,7 +1066,7 @@
         <v>0.96373365462141103</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1084,7 +1092,7 @@
         <v>0.96222876054956796</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -1110,7 +1118,7 @@
         <v>0.969075198019133</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -1136,7 +1144,7 @@
         <v>0.97358414802041804</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -1162,7 +1170,7 @@
         <v>0.96762211776766305</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -1188,7 +1196,7 @@
         <v>0.98477887679313703</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1214,7 +1222,7 @@
         <v>0.97965418136624305</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -1240,7 +1248,7 @@
         <v>0.96939502624238405</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -1266,7 +1274,7 @@
         <v>0.98694183145752501</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -1299,25 +1307,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B1:I44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="11.05078125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="3" width="9.23046875" customWidth="1"/>
-    <col min="4" max="4" width="8.3828125" customWidth="1"/>
-    <col min="5" max="5" width="9.23046875" customWidth="1"/>
-    <col min="6" max="6" width="10.3828125" customWidth="1"/>
-    <col min="7" max="7" width="9.921875" customWidth="1"/>
-    <col min="8" max="8" width="8.3046875" customWidth="1"/>
-    <col min="9" max="9" width="8.61328125" customWidth="1"/>
+    <col min="2" max="2" width="9.05078125" customWidth="1"/>
+    <col min="3" max="3" width="8.41796875" customWidth="1"/>
+    <col min="4" max="4" width="8.05078125" customWidth="1"/>
+    <col min="5" max="5" width="9.20703125" customWidth="1"/>
+    <col min="6" max="6" width="9.15625" customWidth="1"/>
+    <col min="7" max="7" width="8.5234375" customWidth="1"/>
+    <col min="8" max="8" width="8.3125" customWidth="1"/>
+    <col min="9" max="9" width="7.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -1327,7 +1336,7 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="2:9" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -1347,7 +1356,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1367,7 +1376,7 @@
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="1" t="str">
         <f>Raw!B2</f>
         <v>12</v>
@@ -1388,7 +1397,7 @@
         <f>Raw!E2</f>
         <v>0.20821370631456401</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="10">
         <f>Raw!F2</f>
         <v>0.20742366422880501</v>
       </c>
@@ -1401,7 +1410,7 @@
         <v>0.96334564180236104</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="1" t="str">
         <f>Raw!B3</f>
         <v>10</v>
@@ -1411,7 +1420,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D5:D38" si="0">B5*252+B5*C5+C5</f>
+        <f t="shared" ref="D5:D29" si="0">B5*252+B5*C5+C5</f>
         <v>2520</v>
       </c>
       <c r="E5" s="2">
@@ -1422,7 +1431,7 @@
         <f>Raw!E3</f>
         <v>0.208070947229862</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="10">
         <f>Raw!F3</f>
         <v>0.20743071351950601</v>
       </c>
@@ -1435,7 +1444,7 @@
         <v>0.97449145022429995</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="1" t="str">
         <f>Raw!B4</f>
         <v>12</v>
@@ -1456,7 +1465,7 @@
         <f>Raw!E4</f>
         <v>0.208363182842731</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="10">
         <f>Raw!F4</f>
         <v>0.20793694120526299</v>
       </c>
@@ -1469,7 +1478,7 @@
         <v>0.967328027030809</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="1" t="str">
         <f>Raw!B5</f>
         <v>8</v>
@@ -1490,7 +1499,7 @@
         <f>Raw!E5</f>
         <v>0.208266282081604</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="10">
         <f>Raw!F5</f>
         <v>0.208065175578934</v>
       </c>
@@ -1503,7 +1512,7 @@
         <v>0.97009473637974497</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="3" t="str">
         <f>Raw!B6</f>
         <v>10</v>
@@ -1524,7 +1533,7 @@
         <f>Raw!E6</f>
         <v>0.207883018255234</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="11">
         <f>Raw!F6</f>
         <v>0.20832631668492901</v>
       </c>
@@ -1537,7 +1546,7 @@
         <v>0.97349800588123403</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="1" t="str">
         <f>Raw!B7</f>
         <v>14</v>
@@ -1558,7 +1567,7 @@
         <f>Raw!E7</f>
         <v>0.208297699689865</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="10">
         <f>Raw!F7</f>
         <v>0.20856276588766101</v>
       </c>
@@ -1571,7 +1580,7 @@
         <v>0.95788902945036902</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="1" t="str">
         <f>Raw!B8</f>
         <v>14</v>
@@ -1592,7 +1601,7 @@
         <f>Raw!E8</f>
         <v>0.20946079641580601</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="10">
         <f>Raw!F8</f>
         <v>0.20885303442703401</v>
       </c>
@@ -1605,7 +1614,7 @@
         <v>0.96108029067035805</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="1" t="str">
         <f>Raw!B9</f>
         <v>10</v>
@@ -1626,7 +1635,7 @@
         <f>Raw!E9</f>
         <v>0.20896519422531101</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="10">
         <f>Raw!F9</f>
         <v>0.208902506187265</v>
       </c>
@@ -1639,7 +1648,7 @@
         <v>0.97189789350716604</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="1" t="str">
         <f>Raw!B10</f>
         <v>8</v>
@@ -1660,7 +1669,7 @@
         <f>Raw!E10</f>
         <v>0.208391004800797</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="10">
         <f>Raw!F10</f>
         <v>0.20905964355697701</v>
       </c>
@@ -1673,7 +1682,7 @@
         <v>0.97272178501889905</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="3" t="str">
         <f>Raw!B11</f>
         <v>8</v>
@@ -1694,7 +1703,7 @@
         <f>Raw!E11</f>
         <v>0.20962650924921</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="11">
         <f>Raw!F11</f>
         <v>0.20921953026721901</v>
       </c>
@@ -1707,7 +1716,7 @@
         <v>0.97182195896632495</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="1" t="str">
         <f>Raw!B12</f>
         <v>12</v>
@@ -1728,7 +1737,7 @@
         <f>Raw!E12</f>
         <v>0.208155329525471</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="10">
         <f>Raw!F12</f>
         <v>0.20930647366209601</v>
       </c>
@@ -1741,7 +1750,7 @@
         <v>0.96513272317718501</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="1" t="str">
         <f>Raw!B13</f>
         <v>8</v>
@@ -1762,7 +1771,7 @@
         <f>Raw!E13</f>
         <v>0.208521950244904</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="10">
         <f>Raw!F13</f>
         <v>0.20936628967880599</v>
       </c>
@@ -1775,7 +1784,7 @@
         <v>0.97694752227495796</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="1" t="str">
         <f>Raw!B14</f>
         <v>12</v>
@@ -1796,7 +1805,7 @@
         <f>Raw!E14</f>
         <v>0.21032964885234801</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="10">
         <f>Raw!F14</f>
         <v>0.20966253410302099</v>
       </c>
@@ -1809,7 +1818,7 @@
         <v>0.96524418659858802</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="1" t="str">
         <f>Raw!B15</f>
         <v>14</v>
@@ -1830,7 +1839,7 @@
         <f>Raw!E15</f>
         <v>0.21019367724657101</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="10">
         <f>Raw!F15</f>
         <v>0.21057476965902999</v>
       </c>
@@ -1843,7 +1852,7 @@
         <v>0.95918670197864697</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="3" t="str">
         <f>Raw!B16</f>
         <v>10</v>
@@ -1864,7 +1873,7 @@
         <f>Raw!E16</f>
         <v>0.21111193448305099</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="11">
         <f>Raw!F16</f>
         <v>0.21063265053476801</v>
       </c>
@@ -1877,7 +1886,7 @@
         <v>0.97181401875989903</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="1" t="str">
         <f>Raw!B17</f>
         <v>6</v>
@@ -1898,7 +1907,7 @@
         <f>Raw!E17</f>
         <v>0.211464081704617</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="10">
         <f>Raw!F17</f>
         <v>0.21088237977155999</v>
       </c>
@@ -1911,7 +1920,7 @@
         <v>0.97553076110830195</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="1" t="str">
         <f>Raw!B18</f>
         <v>12</v>
@@ -1932,7 +1941,7 @@
         <f>Raw!E18</f>
         <v>0.208563005924225</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="10">
         <f>Raw!F18</f>
         <v>0.21097553393235</v>
       </c>
@@ -1945,7 +1954,7 @@
         <v>0.96373365462141103</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="1" t="str">
         <f>Raw!B19</f>
         <v>14</v>
@@ -1966,7 +1975,7 @@
         <f>Raw!E19</f>
         <v>0.20699615627527199</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="10">
         <f>Raw!F19</f>
         <v>0.21098986984674301</v>
       </c>
@@ -1979,7 +1988,7 @@
         <v>0.96222876054956796</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="1" t="str">
         <f>Raw!B20</f>
         <v>14</v>
@@ -2000,7 +2009,7 @@
         <f>Raw!E20</f>
         <v>0.20861541628837599</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="10">
         <f>Raw!F20</f>
         <v>0.21136462738307901</v>
       </c>
@@ -2013,7 +2022,7 @@
         <v>0.969075198019133</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="3" t="str">
         <f>Raw!B21</f>
         <v>6</v>
@@ -2034,7 +2043,7 @@
         <f>Raw!E21</f>
         <v>0.21424072980880701</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="11">
         <f>Raw!F21</f>
         <v>0.21440788081626699</v>
       </c>
@@ -2047,7 +2056,7 @@
         <v>0.97358414802041804</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="1" t="str">
         <f>Raw!B22</f>
         <v>10</v>
@@ -2068,7 +2077,7 @@
         <f>Raw!E22</f>
         <v>0.21097021400928501</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="10">
         <f>Raw!F22</f>
         <v>0.214887917836491</v>
       </c>
@@ -2081,7 +2090,7 @@
         <v>0.96762211776766305</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="1" t="str">
         <f>Raw!B23</f>
         <v>4</v>
@@ -2102,7 +2111,7 @@
         <f>Raw!E23</f>
         <v>0.21962497085332899</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="10">
         <f>Raw!F23</f>
         <v>0.219443182590458</v>
       </c>
@@ -2115,7 +2124,7 @@
         <v>0.98477887679313703</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" s="1" t="str">
         <f>Raw!B24</f>
         <v>6</v>
@@ -2136,7 +2145,7 @@
         <f>Raw!E24</f>
         <v>0.21892251372337301</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="10">
         <f>Raw!F24</f>
         <v>0.22295899470158401</v>
       </c>
@@ -2149,7 +2158,7 @@
         <v>0.97965418136624305</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" s="1" t="str">
         <f>Raw!B25</f>
         <v>8</v>
@@ -2170,7 +2179,7 @@
         <f>Raw!E25</f>
         <v>0.21933186650276201</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="10">
         <f>Raw!F25</f>
         <v>0.22310107058314199</v>
       </c>
@@ -2183,7 +2192,7 @@
         <v>0.96939502624238405</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="3" t="str">
         <f>Raw!B26</f>
         <v>4</v>
@@ -2204,7 +2213,7 @@
         <f>Raw!E26</f>
         <v>0.224305707216263</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="11">
         <f>Raw!F26</f>
         <v>0.22466951320234799</v>
       </c>
@@ -2217,7 +2226,7 @@
         <v>0.98694183145752501</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="1" t="str">
         <f>Raw!B27</f>
         <v>2</v>
@@ -2238,7 +2247,7 @@
         <f>Raw!E27</f>
         <v>0.23873649090528501</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="10">
         <f>Raw!F27</f>
         <v>0.24050055293276901</v>
       </c>
@@ -2251,7 +2260,7 @@
         <v>0.99245694387044603</v>
       </c>
     </row>
-    <row r="30" spans="2:10" ht="9.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:9" ht="9.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -2261,7 +2270,7 @@
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -2271,95 +2280,87 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="12"/>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="12"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="12"/>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="12"/>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="12"/>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="12"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="12"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="12"/>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -2369,7 +2370,7 @@
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -2379,7 +2380,7 @@
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="2:10" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:9" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -2389,7 +2390,7 @@
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -2399,7 +2400,7 @@
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -2418,7 +2419,7 @@
     <mergeCell ref="D2:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:E44 F4:I4">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2430,6 +2431,54 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F44">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:G44">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:H44">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5:I44">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D41">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -2441,7 +2490,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5:G44">
+  <conditionalFormatting sqref="D4:D29">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2453,8 +2502,44 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:H44">
+  <conditionalFormatting sqref="E4:E29">
     <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:F29">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4:G29">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H29">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2465,8 +2550,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:I44">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="I4:I29">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2477,18 +2562,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D41">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>